<commit_message>
update data download file
</commit_message>
<xml_diff>
--- a/data/Data and Chart Download for Public Spending on Children in Five Charts.xlsx
+++ b/data/Data and Chart Download for Public Spending on Children in Five Charts.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/kidsshare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\LHP\HHahn\Projects\Kids' Share Projects\Kids Share 2018\# Charts for Child Advocates\Download file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="28800" windowHeight="11320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,7 @@
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="126">
   <si>
     <t>Chart 1: Spending on Adults through Social Security, Medicare, and Medicaid Accounted for Nearly Half the Federal Budget in 2017</t>
   </si>
@@ -694,6 +688,42 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">(Washington, DC: Congressional Budget Office, 2018), and Office of Management and Budget, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>Budget of the United States Government,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fiscal Year 2019 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Washington, DC: US Government Printing Office, 2018) and past years. For more source information, </t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="8"/>
@@ -710,7 +740,7 @@
         <rFont val="Lato"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Urban Institute estimates based primarily on Office of Management and Budget, Budget of the </t>
+      <t xml:space="preserve"> Urban Institute estimates based primarily on Office of Management and Budget, </t>
     </r>
   </si>
   <si>
@@ -722,6 +752,37 @@
         <rFont val="Lato"/>
         <family val="2"/>
       </rPr>
+      <t>Source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Urban Institute estimates based primarily on Office of Management and Budget, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Budget of the </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">Source: </t>
     </r>
     <r>
@@ -731,12 +792,7 @@
         <rFont val="Lato"/>
         <family val="2"/>
       </rPr>
-      <t>Urban Institute estimates based primarily on Congressional Budget Office, The Budget and Economic Outlook: 2018 to 2028</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(Washington, DC: Congressional Budget Office, 2018), and Office of Management and Budget, </t>
+      <t xml:space="preserve">Urban Institute estimates based primarily on Congressional Budget Office, </t>
     </r>
     <r>
       <rPr>
@@ -746,59 +802,20 @@
         <rFont val="Lato"/>
         <family val="2"/>
       </rPr>
-      <t>Budget of the United States Government,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Lato"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Fiscal Year 2019 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Lato"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Washington, DC: US Government Printing Office, 2018) and past years. For more source information, </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Lato"/>
-        <family val="2"/>
-      </rPr>
-      <t>Source:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Lato"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Urban Institute estimates based primarily on Office of Management and Budget, </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
+      <t>The Budget and Economic Outlook: 2018 to 2028</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -949,7 +966,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -959,7 +976,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1163,7 +1180,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BDFBCA4-7A22-4726-8306-D5DD06DC39AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BDFBCA4-7A22-4726-8306-D5DD06DC39AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1218,7 +1235,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA95971D-39EA-4E1D-B2B7-24DF99588FCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA95971D-39EA-4E1D-B2B7-24DF99588FCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1273,7 +1290,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61EEB702-A280-49F5-8502-EEDC10DE8CB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61EEB702-A280-49F5-8502-EEDC10DE8CB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1328,7 +1345,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{718E0315-4797-4EEC-97C9-4C6D8720C1C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{718E0315-4797-4EEC-97C9-4C6D8720C1C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1383,7 +1400,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{018562EA-8D63-4F1F-B421-B26967967344}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{018562EA-8D63-4F1F-B421-B26967967344}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1715,70 +1732,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="3"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B9" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1791,46 +1811,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="4.5" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="46.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="41"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1838,7 +1858,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -1846,7 +1866,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -1854,7 +1874,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1882,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -1870,22 +1890,22 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>56</v>
       </c>
@@ -1899,36 +1919,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" style="3" customWidth="1"/>
-    <col min="2" max="8" width="7.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="3" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="45.85546875" style="3" customWidth="1"/>
+    <col min="2" max="8" width="7.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="12" t="s">
         <v>16</v>
@@ -1956,7 +1976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
@@ -1970,7 +1990,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="49"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
@@ -2000,7 +2020,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -2030,7 +2050,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -2060,7 +2080,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -2090,7 +2110,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -2120,12 +2140,12 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="47">
-        <v>0.26</v>
+        <v>0.6</v>
       </c>
       <c r="C10" s="47">
         <v>0.99</v>
@@ -2150,27 +2170,27 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>56</v>
       </c>
@@ -2184,46 +2204,46 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="19" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="40.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="53"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>29</v>
       </c>
@@ -2231,7 +2251,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>30</v>
       </c>
@@ -2239,7 +2259,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>31</v>
       </c>
@@ -2247,7 +2267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>32</v>
       </c>
@@ -2255,7 +2275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>34</v>
       </c>
@@ -2263,7 +2283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>35</v>
       </c>
@@ -2271,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -2279,7 +2299,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>37</v>
       </c>
@@ -2287,7 +2307,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>38</v>
       </c>
@@ -2295,7 +2315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>39</v>
       </c>
@@ -2303,7 +2323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>43</v>
       </c>
@@ -2311,7 +2331,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>40</v>
       </c>
@@ -2319,7 +2339,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>41</v>
       </c>
@@ -2327,7 +2347,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>42</v>
       </c>
@@ -2335,7 +2355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
@@ -2343,7 +2363,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>45</v>
       </c>
@@ -2351,7 +2371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>55</v>
       </c>
@@ -2359,7 +2379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>109</v>
       </c>
@@ -2367,7 +2387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>46</v>
       </c>
@@ -2375,7 +2395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>47</v>
       </c>
@@ -2383,7 +2403,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>48</v>
       </c>
@@ -2391,7 +2411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>49</v>
       </c>
@@ -2399,7 +2419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>50</v>
       </c>
@@ -2407,7 +2427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>51</v>
       </c>
@@ -2415,7 +2435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>52</v>
       </c>
@@ -2423,7 +2443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>53</v>
       </c>
@@ -2431,7 +2451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
@@ -2439,35 +2459,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
         <v>114</v>
       </c>
@@ -2481,35 +2501,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="19" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="15.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="27" t="s">
         <v>58</v>
@@ -2518,14 +2538,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>47</v>
       </c>
@@ -2536,7 +2556,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>36</v>
       </c>
@@ -2547,7 +2567,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>62</v>
       </c>
@@ -2558,32 +2578,32 @@
         <v>2936</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>97</v>
       </c>
@@ -2597,27 +2617,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AL47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="29" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="29" customWidth="1"/>
-    <col min="4" max="8" width="5.5" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="29"/>
+    <col min="1" max="1" width="15.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="29" customWidth="1"/>
+    <col min="4" max="8" width="5.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="29" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:38" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -2636,7 +2656,7 @@
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
     </row>
-    <row r="2" spans="1:38" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:38" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -2655,7 +2675,7 @@
       <c r="N2" s="28"/>
       <c r="O2" s="28"/>
     </row>
-    <row r="3" spans="1:38" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="27" t="s">
         <v>10</v>
@@ -2676,7 +2696,7 @@
       <c r="N3" s="28"/>
       <c r="O3" s="28"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>65</v>
       </c>
@@ -2695,7 +2715,7 @@
       <c r="N4" s="28"/>
       <c r="O4" s="28"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
         <v>66</v>
       </c>
@@ -2741,7 +2761,7 @@
       <c r="AK5" s="38"/>
       <c r="AL5" s="38"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
         <v>67</v>
       </c>
@@ -2764,7 +2784,7 @@
       <c r="N6" s="28"/>
       <c r="O6" s="28"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>68</v>
       </c>
@@ -2787,7 +2807,7 @@
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
         <v>69</v>
       </c>
@@ -2810,7 +2830,7 @@
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
         <v>70</v>
       </c>
@@ -2833,7 +2853,7 @@
       <c r="N9" s="28"/>
       <c r="O9" s="28"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>20</v>
       </c>
@@ -2856,7 +2876,7 @@
       <c r="N10" s="28"/>
       <c r="O10" s="28"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
         <v>71</v>
       </c>
@@ -2879,7 +2899,7 @@
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>72</v>
       </c>
@@ -2902,7 +2922,7 @@
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>73</v>
       </c>
@@ -2925,7 +2945,7 @@
       <c r="N13" s="28"/>
       <c r="O13" s="28"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
@@ -2948,7 +2968,7 @@
       <c r="N14" s="28"/>
       <c r="O14" s="28"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
@@ -2971,7 +2991,7 @@
       <c r="N15" s="28"/>
       <c r="O15" s="28"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
@@ -2994,7 +3014,7 @@
       <c r="N16" s="28"/>
       <c r="O16" s="28"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>77</v>
       </c>
@@ -3017,7 +3037,7 @@
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
         <v>78</v>
       </c>
@@ -3040,7 +3060,7 @@
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>79</v>
       </c>
@@ -3063,7 +3083,7 @@
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>21</v>
       </c>
@@ -3086,7 +3106,7 @@
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>80</v>
       </c>
@@ -3109,7 +3129,7 @@
       <c r="N21" s="28"/>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>81</v>
       </c>
@@ -3132,7 +3152,7 @@
       <c r="N22" s="28"/>
       <c r="O22" s="28"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
         <v>82</v>
       </c>
@@ -3155,7 +3175,7 @@
       <c r="N23" s="28"/>
       <c r="O23" s="28"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
         <v>83</v>
       </c>
@@ -3178,7 +3198,7 @@
       <c r="N24" s="28"/>
       <c r="O24" s="28"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
         <v>84</v>
       </c>
@@ -3201,7 +3221,7 @@
       <c r="N25" s="28"/>
       <c r="O25" s="28"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
         <v>85</v>
       </c>
@@ -3224,7 +3244,7 @@
       <c r="N26" s="28"/>
       <c r="O26" s="28"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
         <v>22</v>
       </c>
@@ -3247,7 +3267,7 @@
       <c r="N27" s="28"/>
       <c r="O27" s="28"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
         <v>86</v>
       </c>
@@ -3270,7 +3290,7 @@
       <c r="N28" s="28"/>
       <c r="O28" s="28"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
         <v>87</v>
       </c>
@@ -3293,7 +3313,7 @@
       <c r="N29" s="28"/>
       <c r="O29" s="28"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
         <v>88</v>
       </c>
@@ -3316,7 +3336,7 @@
       <c r="N30" s="28"/>
       <c r="O30" s="28"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
         <v>89</v>
       </c>
@@ -3339,7 +3359,7 @@
       <c r="N31" s="28"/>
       <c r="O31" s="28"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
         <v>90</v>
       </c>
@@ -3362,7 +3382,7 @@
       <c r="N32" s="28"/>
       <c r="O32" s="28"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
         <v>91</v>
       </c>
@@ -3385,7 +3405,7 @@
       <c r="N33" s="28"/>
       <c r="O33" s="28"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
         <v>92</v>
       </c>
@@ -3408,7 +3428,7 @@
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
         <v>93</v>
       </c>
@@ -3431,7 +3451,7 @@
       <c r="N35" s="28"/>
       <c r="O35" s="28"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
         <v>94</v>
       </c>
@@ -3454,7 +3474,7 @@
       <c r="N36" s="28"/>
       <c r="O36" s="28"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
         <v>95</v>
       </c>
@@ -3477,7 +3497,7 @@
       <c r="N37" s="28"/>
       <c r="O37" s="28"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>23</v>
       </c>
@@ -3500,7 +3520,7 @@
       <c r="N38" s="28"/>
       <c r="O38" s="28"/>
     </row>
-    <row r="39" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
         <v>118</v>
       </c>
@@ -3519,7 +3539,7 @@
       <c r="N39" s="28"/>
       <c r="O39" s="28"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="s">
         <v>103</v>
       </c>
@@ -3538,7 +3558,7 @@
       <c r="N40" s="28"/>
       <c r="O40" s="28"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
         <v>104</v>
       </c>
@@ -3557,7 +3577,7 @@
       <c r="N41" s="28"/>
       <c r="O41" s="28"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="24" t="s">
         <v>105</v>
       </c>
@@ -3576,7 +3596,7 @@
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="40" t="s">
         <v>106</v>
       </c>
@@ -3595,7 +3615,7 @@
       <c r="N43" s="28"/>
       <c r="O43" s="28"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="24" t="s">
         <v>107</v>
       </c>
@@ -3614,7 +3634,7 @@
       <c r="N44" s="28"/>
       <c r="O44" s="28"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
         <v>108</v>
       </c>
@@ -3633,7 +3653,7 @@
       <c r="N45" s="28"/>
       <c r="O45" s="28"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
@@ -3650,7 +3670,7 @@
       <c r="N46" s="28"/>
       <c r="O46" s="28"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="28"/>
       <c r="B47" s="28"/>
       <c r="C47" s="28"/>

</xml_diff>